<commit_message>
ins 10/02 17:45 :# Ple ase enter the commit message for your changes. Lines starting
</commit_message>
<xml_diff>
--- a/020-内部_プログラミング設計/021-クラス図/商品検索機能/021-クラス図_商品検索画面.xlsx
+++ b/020-内部_プログラミング設計/021-クラス図/商品検索機能/021-クラス図_商品検索画面.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\システム開発演習\020-内部_プログラミング設計\021-クラス図\商品検索機能\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D7E9B41-F49D-4D79-8F0B-7430057CD0BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7134139E-DECD-4421-9624-3BD39948A77F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="表紙" sheetId="10" r:id="rId1"/>
@@ -802,11 +802,53 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -844,63 +886,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -923,6 +910,19 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="26" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="30" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
@@ -1137,21 +1137,21 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>71846</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>61</xdr:col>
-      <xdr:colOff>172934</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>9657</xdr:rowOff>
+      <xdr:col>70</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>102546</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="図 2">
+        <xdr:cNvPr id="4" name="図 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF29C87B-47AA-445F-B5AC-EC480115B6BE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB22E35E-96C0-458C-9205-DAACAF372035}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1167,15 +1167,15 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="1160417"/>
-          <a:ext cx="10973195" cy="8971049"/>
+          <a:off x="0" y="1219200"/>
+          <a:ext cx="13354050" cy="10218096"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln w="38100">
+        <a:ln w="28575">
           <a:solidFill>
-            <a:schemeClr val="tx1"/>
+            <a:sysClr val="windowText" lastClr="000000"/>
           </a:solidFill>
         </a:ln>
       </xdr:spPr>
@@ -1679,23 +1679,23 @@
     </row>
     <row r="3" spans="1:52" ht="10.5" customHeight="1">
       <c r="A3" s="5"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="43"/>
-      <c r="M3" s="45" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
-      <c r="P3" s="45"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
       <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
@@ -1711,49 +1711,49 @@
       <c r="AC3" s="6"/>
       <c r="AD3" s="6"/>
       <c r="AE3" s="6"/>
-      <c r="AF3" s="29" t="s">
+      <c r="AF3" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="AG3" s="29"/>
-      <c r="AH3" s="29"/>
-      <c r="AI3" s="29"/>
-      <c r="AJ3" s="29"/>
-      <c r="AK3" s="29"/>
-      <c r="AL3" s="42" t="s">
+      <c r="AG3" s="32"/>
+      <c r="AH3" s="32"/>
+      <c r="AI3" s="32"/>
+      <c r="AJ3" s="32"/>
+      <c r="AK3" s="32"/>
+      <c r="AL3" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="AM3" s="42"/>
-      <c r="AN3" s="42"/>
-      <c r="AO3" s="42"/>
-      <c r="AP3" s="42"/>
-      <c r="AQ3" s="42"/>
-      <c r="AR3" s="42"/>
-      <c r="AS3" s="42"/>
-      <c r="AT3" s="42"/>
-      <c r="AU3" s="42"/>
-      <c r="AV3" s="42"/>
-      <c r="AW3" s="42"/>
-      <c r="AX3" s="42"/>
-      <c r="AY3" s="42"/>
+      <c r="AM3" s="33"/>
+      <c r="AN3" s="33"/>
+      <c r="AO3" s="33"/>
+      <c r="AP3" s="33"/>
+      <c r="AQ3" s="33"/>
+      <c r="AR3" s="33"/>
+      <c r="AS3" s="33"/>
+      <c r="AT3" s="33"/>
+      <c r="AU3" s="33"/>
+      <c r="AV3" s="33"/>
+      <c r="AW3" s="33"/>
+      <c r="AX3" s="33"/>
+      <c r="AY3" s="33"/>
       <c r="AZ3" s="7"/>
     </row>
     <row r="4" spans="1:52" ht="10.5" customHeight="1">
       <c r="A4" s="5"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="46"/>
-      <c r="O4" s="46"/>
-      <c r="P4" s="46"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
@@ -1769,26 +1769,26 @@
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
       <c r="AE4" s="6"/>
-      <c r="AF4" s="29"/>
-      <c r="AG4" s="29"/>
-      <c r="AH4" s="29"/>
-      <c r="AI4" s="29"/>
-      <c r="AJ4" s="29"/>
-      <c r="AK4" s="29"/>
-      <c r="AL4" s="42"/>
-      <c r="AM4" s="42"/>
-      <c r="AN4" s="42"/>
-      <c r="AO4" s="42"/>
-      <c r="AP4" s="42"/>
-      <c r="AQ4" s="42"/>
-      <c r="AR4" s="42"/>
-      <c r="AS4" s="42"/>
-      <c r="AT4" s="42"/>
-      <c r="AU4" s="42"/>
-      <c r="AV4" s="42"/>
-      <c r="AW4" s="42"/>
-      <c r="AX4" s="42"/>
-      <c r="AY4" s="42"/>
+      <c r="AF4" s="32"/>
+      <c r="AG4" s="32"/>
+      <c r="AH4" s="32"/>
+      <c r="AI4" s="32"/>
+      <c r="AJ4" s="32"/>
+      <c r="AK4" s="32"/>
+      <c r="AL4" s="33"/>
+      <c r="AM4" s="33"/>
+      <c r="AN4" s="33"/>
+      <c r="AO4" s="33"/>
+      <c r="AP4" s="33"/>
+      <c r="AQ4" s="33"/>
+      <c r="AR4" s="33"/>
+      <c r="AS4" s="33"/>
+      <c r="AT4" s="33"/>
+      <c r="AU4" s="33"/>
+      <c r="AV4" s="33"/>
+      <c r="AW4" s="33"/>
+      <c r="AX4" s="33"/>
+      <c r="AY4" s="33"/>
       <c r="AZ4" s="7"/>
     </row>
     <row r="5" spans="1:52" ht="10.5" customHeight="1">
@@ -2394,44 +2394,44 @@
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
-      <c r="I16" s="47" t="s">
+      <c r="I16" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="J16" s="48"/>
-      <c r="K16" s="48"/>
-      <c r="L16" s="48"/>
-      <c r="M16" s="48"/>
-      <c r="N16" s="48"/>
-      <c r="O16" s="48"/>
-      <c r="P16" s="48"/>
-      <c r="Q16" s="48"/>
-      <c r="R16" s="48"/>
-      <c r="S16" s="48"/>
-      <c r="T16" s="48"/>
-      <c r="U16" s="48"/>
-      <c r="V16" s="48"/>
-      <c r="W16" s="48"/>
-      <c r="X16" s="48"/>
-      <c r="Y16" s="48"/>
-      <c r="Z16" s="48"/>
-      <c r="AA16" s="48"/>
-      <c r="AB16" s="48"/>
-      <c r="AC16" s="48"/>
-      <c r="AD16" s="48"/>
-      <c r="AE16" s="48"/>
-      <c r="AF16" s="48"/>
-      <c r="AG16" s="48"/>
-      <c r="AH16" s="48"/>
-      <c r="AI16" s="48"/>
-      <c r="AJ16" s="48"/>
-      <c r="AK16" s="48"/>
-      <c r="AL16" s="48"/>
-      <c r="AM16" s="48"/>
-      <c r="AN16" s="48"/>
-      <c r="AO16" s="48"/>
-      <c r="AP16" s="48"/>
-      <c r="AQ16" s="48"/>
-      <c r="AR16" s="49"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="35"/>
+      <c r="O16" s="35"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="35"/>
+      <c r="R16" s="35"/>
+      <c r="S16" s="35"/>
+      <c r="T16" s="35"/>
+      <c r="U16" s="35"/>
+      <c r="V16" s="35"/>
+      <c r="W16" s="35"/>
+      <c r="X16" s="35"/>
+      <c r="Y16" s="35"/>
+      <c r="Z16" s="35"/>
+      <c r="AA16" s="35"/>
+      <c r="AB16" s="35"/>
+      <c r="AC16" s="35"/>
+      <c r="AD16" s="35"/>
+      <c r="AE16" s="35"/>
+      <c r="AF16" s="35"/>
+      <c r="AG16" s="35"/>
+      <c r="AH16" s="35"/>
+      <c r="AI16" s="35"/>
+      <c r="AJ16" s="35"/>
+      <c r="AK16" s="35"/>
+      <c r="AL16" s="35"/>
+      <c r="AM16" s="35"/>
+      <c r="AN16" s="35"/>
+      <c r="AO16" s="35"/>
+      <c r="AP16" s="35"/>
+      <c r="AQ16" s="35"/>
+      <c r="AR16" s="36"/>
       <c r="AS16" s="10"/>
       <c r="AT16" s="10"/>
       <c r="AU16" s="10"/>
@@ -2450,42 +2450,42 @@
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="51"/>
-      <c r="N17" s="51"/>
-      <c r="O17" s="51"/>
-      <c r="P17" s="51"/>
-      <c r="Q17" s="51"/>
-      <c r="R17" s="51"/>
-      <c r="S17" s="51"/>
-      <c r="T17" s="51"/>
-      <c r="U17" s="51"/>
-      <c r="V17" s="51"/>
-      <c r="W17" s="51"/>
-      <c r="X17" s="51"/>
-      <c r="Y17" s="51"/>
-      <c r="Z17" s="51"/>
-      <c r="AA17" s="51"/>
-      <c r="AB17" s="51"/>
-      <c r="AC17" s="51"/>
-      <c r="AD17" s="51"/>
-      <c r="AE17" s="51"/>
-      <c r="AF17" s="51"/>
-      <c r="AG17" s="51"/>
-      <c r="AH17" s="51"/>
-      <c r="AI17" s="51"/>
-      <c r="AJ17" s="51"/>
-      <c r="AK17" s="51"/>
-      <c r="AL17" s="51"/>
-      <c r="AM17" s="51"/>
-      <c r="AN17" s="51"/>
-      <c r="AO17" s="51"/>
-      <c r="AP17" s="51"/>
-      <c r="AQ17" s="51"/>
-      <c r="AR17" s="52"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="38"/>
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="38"/>
+      <c r="O17" s="38"/>
+      <c r="P17" s="38"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="38"/>
+      <c r="S17" s="38"/>
+      <c r="T17" s="38"/>
+      <c r="U17" s="38"/>
+      <c r="V17" s="38"/>
+      <c r="W17" s="38"/>
+      <c r="X17" s="38"/>
+      <c r="Y17" s="38"/>
+      <c r="Z17" s="38"/>
+      <c r="AA17" s="38"/>
+      <c r="AB17" s="38"/>
+      <c r="AC17" s="38"/>
+      <c r="AD17" s="38"/>
+      <c r="AE17" s="38"/>
+      <c r="AF17" s="38"/>
+      <c r="AG17" s="38"/>
+      <c r="AH17" s="38"/>
+      <c r="AI17" s="38"/>
+      <c r="AJ17" s="38"/>
+      <c r="AK17" s="38"/>
+      <c r="AL17" s="38"/>
+      <c r="AM17" s="38"/>
+      <c r="AN17" s="38"/>
+      <c r="AO17" s="38"/>
+      <c r="AP17" s="38"/>
+      <c r="AQ17" s="38"/>
+      <c r="AR17" s="39"/>
       <c r="AS17" s="10"/>
       <c r="AT17" s="10"/>
       <c r="AU17" s="10"/>
@@ -2504,42 +2504,42 @@
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="51"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="51"/>
-      <c r="M18" s="51"/>
-      <c r="N18" s="51"/>
-      <c r="O18" s="51"/>
-      <c r="P18" s="51"/>
-      <c r="Q18" s="51"/>
-      <c r="R18" s="51"/>
-      <c r="S18" s="51"/>
-      <c r="T18" s="51"/>
-      <c r="U18" s="51"/>
-      <c r="V18" s="51"/>
-      <c r="W18" s="51"/>
-      <c r="X18" s="51"/>
-      <c r="Y18" s="51"/>
-      <c r="Z18" s="51"/>
-      <c r="AA18" s="51"/>
-      <c r="AB18" s="51"/>
-      <c r="AC18" s="51"/>
-      <c r="AD18" s="51"/>
-      <c r="AE18" s="51"/>
-      <c r="AF18" s="51"/>
-      <c r="AG18" s="51"/>
-      <c r="AH18" s="51"/>
-      <c r="AI18" s="51"/>
-      <c r="AJ18" s="51"/>
-      <c r="AK18" s="51"/>
-      <c r="AL18" s="51"/>
-      <c r="AM18" s="51"/>
-      <c r="AN18" s="51"/>
-      <c r="AO18" s="51"/>
-      <c r="AP18" s="51"/>
-      <c r="AQ18" s="51"/>
-      <c r="AR18" s="52"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
+      <c r="P18" s="38"/>
+      <c r="Q18" s="38"/>
+      <c r="R18" s="38"/>
+      <c r="S18" s="38"/>
+      <c r="T18" s="38"/>
+      <c r="U18" s="38"/>
+      <c r="V18" s="38"/>
+      <c r="W18" s="38"/>
+      <c r="X18" s="38"/>
+      <c r="Y18" s="38"/>
+      <c r="Z18" s="38"/>
+      <c r="AA18" s="38"/>
+      <c r="AB18" s="38"/>
+      <c r="AC18" s="38"/>
+      <c r="AD18" s="38"/>
+      <c r="AE18" s="38"/>
+      <c r="AF18" s="38"/>
+      <c r="AG18" s="38"/>
+      <c r="AH18" s="38"/>
+      <c r="AI18" s="38"/>
+      <c r="AJ18" s="38"/>
+      <c r="AK18" s="38"/>
+      <c r="AL18" s="38"/>
+      <c r="AM18" s="38"/>
+      <c r="AN18" s="38"/>
+      <c r="AO18" s="38"/>
+      <c r="AP18" s="38"/>
+      <c r="AQ18" s="38"/>
+      <c r="AR18" s="39"/>
       <c r="AS18" s="10"/>
       <c r="AT18" s="10"/>
       <c r="AU18" s="10"/>
@@ -2558,42 +2558,42 @@
       <c r="F19" s="10"/>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="51"/>
-      <c r="P19" s="51"/>
-      <c r="Q19" s="51"/>
-      <c r="R19" s="51"/>
-      <c r="S19" s="51"/>
-      <c r="T19" s="51"/>
-      <c r="U19" s="51"/>
-      <c r="V19" s="51"/>
-      <c r="W19" s="51"/>
-      <c r="X19" s="51"/>
-      <c r="Y19" s="51"/>
-      <c r="Z19" s="51"/>
-      <c r="AA19" s="51"/>
-      <c r="AB19" s="51"/>
-      <c r="AC19" s="51"/>
-      <c r="AD19" s="51"/>
-      <c r="AE19" s="51"/>
-      <c r="AF19" s="51"/>
-      <c r="AG19" s="51"/>
-      <c r="AH19" s="51"/>
-      <c r="AI19" s="51"/>
-      <c r="AJ19" s="51"/>
-      <c r="AK19" s="51"/>
-      <c r="AL19" s="51"/>
-      <c r="AM19" s="51"/>
-      <c r="AN19" s="51"/>
-      <c r="AO19" s="51"/>
-      <c r="AP19" s="51"/>
-      <c r="AQ19" s="51"/>
-      <c r="AR19" s="52"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="38"/>
+      <c r="P19" s="38"/>
+      <c r="Q19" s="38"/>
+      <c r="R19" s="38"/>
+      <c r="S19" s="38"/>
+      <c r="T19" s="38"/>
+      <c r="U19" s="38"/>
+      <c r="V19" s="38"/>
+      <c r="W19" s="38"/>
+      <c r="X19" s="38"/>
+      <c r="Y19" s="38"/>
+      <c r="Z19" s="38"/>
+      <c r="AA19" s="38"/>
+      <c r="AB19" s="38"/>
+      <c r="AC19" s="38"/>
+      <c r="AD19" s="38"/>
+      <c r="AE19" s="38"/>
+      <c r="AF19" s="38"/>
+      <c r="AG19" s="38"/>
+      <c r="AH19" s="38"/>
+      <c r="AI19" s="38"/>
+      <c r="AJ19" s="38"/>
+      <c r="AK19" s="38"/>
+      <c r="AL19" s="38"/>
+      <c r="AM19" s="38"/>
+      <c r="AN19" s="38"/>
+      <c r="AO19" s="38"/>
+      <c r="AP19" s="38"/>
+      <c r="AQ19" s="38"/>
+      <c r="AR19" s="39"/>
       <c r="AS19" s="10"/>
       <c r="AT19" s="10"/>
       <c r="AU19" s="10"/>
@@ -2612,42 +2612,42 @@
       <c r="F20" s="10"/>
       <c r="G20" s="10"/>
       <c r="H20" s="10"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="51"/>
-      <c r="K20" s="51"/>
-      <c r="L20" s="51"/>
-      <c r="M20" s="51"/>
-      <c r="N20" s="51"/>
-      <c r="O20" s="51"/>
-      <c r="P20" s="51"/>
-      <c r="Q20" s="51"/>
-      <c r="R20" s="51"/>
-      <c r="S20" s="51"/>
-      <c r="T20" s="51"/>
-      <c r="U20" s="51"/>
-      <c r="V20" s="51"/>
-      <c r="W20" s="51"/>
-      <c r="X20" s="51"/>
-      <c r="Y20" s="51"/>
-      <c r="Z20" s="51"/>
-      <c r="AA20" s="51"/>
-      <c r="AB20" s="51"/>
-      <c r="AC20" s="51"/>
-      <c r="AD20" s="51"/>
-      <c r="AE20" s="51"/>
-      <c r="AF20" s="51"/>
-      <c r="AG20" s="51"/>
-      <c r="AH20" s="51"/>
-      <c r="AI20" s="51"/>
-      <c r="AJ20" s="51"/>
-      <c r="AK20" s="51"/>
-      <c r="AL20" s="51"/>
-      <c r="AM20" s="51"/>
-      <c r="AN20" s="51"/>
-      <c r="AO20" s="51"/>
-      <c r="AP20" s="51"/>
-      <c r="AQ20" s="51"/>
-      <c r="AR20" s="52"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="38"/>
+      <c r="P20" s="38"/>
+      <c r="Q20" s="38"/>
+      <c r="R20" s="38"/>
+      <c r="S20" s="38"/>
+      <c r="T20" s="38"/>
+      <c r="U20" s="38"/>
+      <c r="V20" s="38"/>
+      <c r="W20" s="38"/>
+      <c r="X20" s="38"/>
+      <c r="Y20" s="38"/>
+      <c r="Z20" s="38"/>
+      <c r="AA20" s="38"/>
+      <c r="AB20" s="38"/>
+      <c r="AC20" s="38"/>
+      <c r="AD20" s="38"/>
+      <c r="AE20" s="38"/>
+      <c r="AF20" s="38"/>
+      <c r="AG20" s="38"/>
+      <c r="AH20" s="38"/>
+      <c r="AI20" s="38"/>
+      <c r="AJ20" s="38"/>
+      <c r="AK20" s="38"/>
+      <c r="AL20" s="38"/>
+      <c r="AM20" s="38"/>
+      <c r="AN20" s="38"/>
+      <c r="AO20" s="38"/>
+      <c r="AP20" s="38"/>
+      <c r="AQ20" s="38"/>
+      <c r="AR20" s="39"/>
       <c r="AS20" s="10"/>
       <c r="AT20" s="10"/>
       <c r="AU20" s="10"/>
@@ -2666,42 +2666,42 @@
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="51"/>
-      <c r="K21" s="51"/>
-      <c r="L21" s="51"/>
-      <c r="M21" s="51"/>
-      <c r="N21" s="51"/>
-      <c r="O21" s="51"/>
-      <c r="P21" s="51"/>
-      <c r="Q21" s="51"/>
-      <c r="R21" s="51"/>
-      <c r="S21" s="51"/>
-      <c r="T21" s="51"/>
-      <c r="U21" s="51"/>
-      <c r="V21" s="51"/>
-      <c r="W21" s="51"/>
-      <c r="X21" s="51"/>
-      <c r="Y21" s="51"/>
-      <c r="Z21" s="51"/>
-      <c r="AA21" s="51"/>
-      <c r="AB21" s="51"/>
-      <c r="AC21" s="51"/>
-      <c r="AD21" s="51"/>
-      <c r="AE21" s="51"/>
-      <c r="AF21" s="51"/>
-      <c r="AG21" s="51"/>
-      <c r="AH21" s="51"/>
-      <c r="AI21" s="51"/>
-      <c r="AJ21" s="51"/>
-      <c r="AK21" s="51"/>
-      <c r="AL21" s="51"/>
-      <c r="AM21" s="51"/>
-      <c r="AN21" s="51"/>
-      <c r="AO21" s="51"/>
-      <c r="AP21" s="51"/>
-      <c r="AQ21" s="51"/>
-      <c r="AR21" s="52"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="38"/>
+      <c r="P21" s="38"/>
+      <c r="Q21" s="38"/>
+      <c r="R21" s="38"/>
+      <c r="S21" s="38"/>
+      <c r="T21" s="38"/>
+      <c r="U21" s="38"/>
+      <c r="V21" s="38"/>
+      <c r="W21" s="38"/>
+      <c r="X21" s="38"/>
+      <c r="Y21" s="38"/>
+      <c r="Z21" s="38"/>
+      <c r="AA21" s="38"/>
+      <c r="AB21" s="38"/>
+      <c r="AC21" s="38"/>
+      <c r="AD21" s="38"/>
+      <c r="AE21" s="38"/>
+      <c r="AF21" s="38"/>
+      <c r="AG21" s="38"/>
+      <c r="AH21" s="38"/>
+      <c r="AI21" s="38"/>
+      <c r="AJ21" s="38"/>
+      <c r="AK21" s="38"/>
+      <c r="AL21" s="38"/>
+      <c r="AM21" s="38"/>
+      <c r="AN21" s="38"/>
+      <c r="AO21" s="38"/>
+      <c r="AP21" s="38"/>
+      <c r="AQ21" s="38"/>
+      <c r="AR21" s="39"/>
       <c r="AS21" s="10"/>
       <c r="AT21" s="10"/>
       <c r="AU21" s="10"/>
@@ -2720,42 +2720,42 @@
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
       <c r="H22" s="10"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="51"/>
-      <c r="L22" s="51"/>
-      <c r="M22" s="51"/>
-      <c r="N22" s="51"/>
-      <c r="O22" s="51"/>
-      <c r="P22" s="51"/>
-      <c r="Q22" s="51"/>
-      <c r="R22" s="51"/>
-      <c r="S22" s="51"/>
-      <c r="T22" s="51"/>
-      <c r="U22" s="51"/>
-      <c r="V22" s="51"/>
-      <c r="W22" s="51"/>
-      <c r="X22" s="51"/>
-      <c r="Y22" s="51"/>
-      <c r="Z22" s="51"/>
-      <c r="AA22" s="51"/>
-      <c r="AB22" s="51"/>
-      <c r="AC22" s="51"/>
-      <c r="AD22" s="51"/>
-      <c r="AE22" s="51"/>
-      <c r="AF22" s="51"/>
-      <c r="AG22" s="51"/>
-      <c r="AH22" s="51"/>
-      <c r="AI22" s="51"/>
-      <c r="AJ22" s="51"/>
-      <c r="AK22" s="51"/>
-      <c r="AL22" s="51"/>
-      <c r="AM22" s="51"/>
-      <c r="AN22" s="51"/>
-      <c r="AO22" s="51"/>
-      <c r="AP22" s="51"/>
-      <c r="AQ22" s="51"/>
-      <c r="AR22" s="52"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="38"/>
+      <c r="P22" s="38"/>
+      <c r="Q22" s="38"/>
+      <c r="R22" s="38"/>
+      <c r="S22" s="38"/>
+      <c r="T22" s="38"/>
+      <c r="U22" s="38"/>
+      <c r="V22" s="38"/>
+      <c r="W22" s="38"/>
+      <c r="X22" s="38"/>
+      <c r="Y22" s="38"/>
+      <c r="Z22" s="38"/>
+      <c r="AA22" s="38"/>
+      <c r="AB22" s="38"/>
+      <c r="AC22" s="38"/>
+      <c r="AD22" s="38"/>
+      <c r="AE22" s="38"/>
+      <c r="AF22" s="38"/>
+      <c r="AG22" s="38"/>
+      <c r="AH22" s="38"/>
+      <c r="AI22" s="38"/>
+      <c r="AJ22" s="38"/>
+      <c r="AK22" s="38"/>
+      <c r="AL22" s="38"/>
+      <c r="AM22" s="38"/>
+      <c r="AN22" s="38"/>
+      <c r="AO22" s="38"/>
+      <c r="AP22" s="38"/>
+      <c r="AQ22" s="38"/>
+      <c r="AR22" s="39"/>
       <c r="AS22" s="10"/>
       <c r="AT22" s="10"/>
       <c r="AU22" s="10"/>
@@ -2774,42 +2774,42 @@
       <c r="F23" s="10"/>
       <c r="G23" s="10"/>
       <c r="H23" s="10"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="51"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="51"/>
-      <c r="M23" s="51"/>
-      <c r="N23" s="51"/>
-      <c r="O23" s="51"/>
-      <c r="P23" s="51"/>
-      <c r="Q23" s="51"/>
-      <c r="R23" s="51"/>
-      <c r="S23" s="51"/>
-      <c r="T23" s="51"/>
-      <c r="U23" s="51"/>
-      <c r="V23" s="51"/>
-      <c r="W23" s="51"/>
-      <c r="X23" s="51"/>
-      <c r="Y23" s="51"/>
-      <c r="Z23" s="51"/>
-      <c r="AA23" s="51"/>
-      <c r="AB23" s="51"/>
-      <c r="AC23" s="51"/>
-      <c r="AD23" s="51"/>
-      <c r="AE23" s="51"/>
-      <c r="AF23" s="51"/>
-      <c r="AG23" s="51"/>
-      <c r="AH23" s="51"/>
-      <c r="AI23" s="51"/>
-      <c r="AJ23" s="51"/>
-      <c r="AK23" s="51"/>
-      <c r="AL23" s="51"/>
-      <c r="AM23" s="51"/>
-      <c r="AN23" s="51"/>
-      <c r="AO23" s="51"/>
-      <c r="AP23" s="51"/>
-      <c r="AQ23" s="51"/>
-      <c r="AR23" s="52"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="38"/>
+      <c r="O23" s="38"/>
+      <c r="P23" s="38"/>
+      <c r="Q23" s="38"/>
+      <c r="R23" s="38"/>
+      <c r="S23" s="38"/>
+      <c r="T23" s="38"/>
+      <c r="U23" s="38"/>
+      <c r="V23" s="38"/>
+      <c r="W23" s="38"/>
+      <c r="X23" s="38"/>
+      <c r="Y23" s="38"/>
+      <c r="Z23" s="38"/>
+      <c r="AA23" s="38"/>
+      <c r="AB23" s="38"/>
+      <c r="AC23" s="38"/>
+      <c r="AD23" s="38"/>
+      <c r="AE23" s="38"/>
+      <c r="AF23" s="38"/>
+      <c r="AG23" s="38"/>
+      <c r="AH23" s="38"/>
+      <c r="AI23" s="38"/>
+      <c r="AJ23" s="38"/>
+      <c r="AK23" s="38"/>
+      <c r="AL23" s="38"/>
+      <c r="AM23" s="38"/>
+      <c r="AN23" s="38"/>
+      <c r="AO23" s="38"/>
+      <c r="AP23" s="38"/>
+      <c r="AQ23" s="38"/>
+      <c r="AR23" s="39"/>
       <c r="AS23" s="10"/>
       <c r="AT23" s="10"/>
       <c r="AU23" s="10"/>
@@ -2828,42 +2828,42 @@
       <c r="F24" s="10"/>
       <c r="G24" s="10"/>
       <c r="H24" s="10"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="51"/>
-      <c r="K24" s="51"/>
-      <c r="L24" s="51"/>
-      <c r="M24" s="51"/>
-      <c r="N24" s="51"/>
-      <c r="O24" s="51"/>
-      <c r="P24" s="51"/>
-      <c r="Q24" s="51"/>
-      <c r="R24" s="51"/>
-      <c r="S24" s="51"/>
-      <c r="T24" s="51"/>
-      <c r="U24" s="51"/>
-      <c r="V24" s="51"/>
-      <c r="W24" s="51"/>
-      <c r="X24" s="51"/>
-      <c r="Y24" s="51"/>
-      <c r="Z24" s="51"/>
-      <c r="AA24" s="51"/>
-      <c r="AB24" s="51"/>
-      <c r="AC24" s="51"/>
-      <c r="AD24" s="51"/>
-      <c r="AE24" s="51"/>
-      <c r="AF24" s="51"/>
-      <c r="AG24" s="51"/>
-      <c r="AH24" s="51"/>
-      <c r="AI24" s="51"/>
-      <c r="AJ24" s="51"/>
-      <c r="AK24" s="51"/>
-      <c r="AL24" s="51"/>
-      <c r="AM24" s="51"/>
-      <c r="AN24" s="51"/>
-      <c r="AO24" s="51"/>
-      <c r="AP24" s="51"/>
-      <c r="AQ24" s="51"/>
-      <c r="AR24" s="52"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="38"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="38"/>
+      <c r="P24" s="38"/>
+      <c r="Q24" s="38"/>
+      <c r="R24" s="38"/>
+      <c r="S24" s="38"/>
+      <c r="T24" s="38"/>
+      <c r="U24" s="38"/>
+      <c r="V24" s="38"/>
+      <c r="W24" s="38"/>
+      <c r="X24" s="38"/>
+      <c r="Y24" s="38"/>
+      <c r="Z24" s="38"/>
+      <c r="AA24" s="38"/>
+      <c r="AB24" s="38"/>
+      <c r="AC24" s="38"/>
+      <c r="AD24" s="38"/>
+      <c r="AE24" s="38"/>
+      <c r="AF24" s="38"/>
+      <c r="AG24" s="38"/>
+      <c r="AH24" s="38"/>
+      <c r="AI24" s="38"/>
+      <c r="AJ24" s="38"/>
+      <c r="AK24" s="38"/>
+      <c r="AL24" s="38"/>
+      <c r="AM24" s="38"/>
+      <c r="AN24" s="38"/>
+      <c r="AO24" s="38"/>
+      <c r="AP24" s="38"/>
+      <c r="AQ24" s="38"/>
+      <c r="AR24" s="39"/>
       <c r="AS24" s="10"/>
       <c r="AT24" s="10"/>
       <c r="AU24" s="10"/>
@@ -2882,42 +2882,42 @@
       <c r="F25" s="10"/>
       <c r="G25" s="10"/>
       <c r="H25" s="10"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="51"/>
-      <c r="K25" s="51"/>
-      <c r="L25" s="51"/>
-      <c r="M25" s="51"/>
-      <c r="N25" s="51"/>
-      <c r="O25" s="51"/>
-      <c r="P25" s="51"/>
-      <c r="Q25" s="51"/>
-      <c r="R25" s="51"/>
-      <c r="S25" s="51"/>
-      <c r="T25" s="51"/>
-      <c r="U25" s="51"/>
-      <c r="V25" s="51"/>
-      <c r="W25" s="51"/>
-      <c r="X25" s="51"/>
-      <c r="Y25" s="51"/>
-      <c r="Z25" s="51"/>
-      <c r="AA25" s="51"/>
-      <c r="AB25" s="51"/>
-      <c r="AC25" s="51"/>
-      <c r="AD25" s="51"/>
-      <c r="AE25" s="51"/>
-      <c r="AF25" s="51"/>
-      <c r="AG25" s="51"/>
-      <c r="AH25" s="51"/>
-      <c r="AI25" s="51"/>
-      <c r="AJ25" s="51"/>
-      <c r="AK25" s="51"/>
-      <c r="AL25" s="51"/>
-      <c r="AM25" s="51"/>
-      <c r="AN25" s="51"/>
-      <c r="AO25" s="51"/>
-      <c r="AP25" s="51"/>
-      <c r="AQ25" s="51"/>
-      <c r="AR25" s="52"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="38"/>
+      <c r="N25" s="38"/>
+      <c r="O25" s="38"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="38"/>
+      <c r="S25" s="38"/>
+      <c r="T25" s="38"/>
+      <c r="U25" s="38"/>
+      <c r="V25" s="38"/>
+      <c r="W25" s="38"/>
+      <c r="X25" s="38"/>
+      <c r="Y25" s="38"/>
+      <c r="Z25" s="38"/>
+      <c r="AA25" s="38"/>
+      <c r="AB25" s="38"/>
+      <c r="AC25" s="38"/>
+      <c r="AD25" s="38"/>
+      <c r="AE25" s="38"/>
+      <c r="AF25" s="38"/>
+      <c r="AG25" s="38"/>
+      <c r="AH25" s="38"/>
+      <c r="AI25" s="38"/>
+      <c r="AJ25" s="38"/>
+      <c r="AK25" s="38"/>
+      <c r="AL25" s="38"/>
+      <c r="AM25" s="38"/>
+      <c r="AN25" s="38"/>
+      <c r="AO25" s="38"/>
+      <c r="AP25" s="38"/>
+      <c r="AQ25" s="38"/>
+      <c r="AR25" s="39"/>
       <c r="AS25" s="10"/>
       <c r="AT25" s="10"/>
       <c r="AU25" s="10"/>
@@ -2936,42 +2936,42 @@
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="51"/>
-      <c r="K26" s="51"/>
-      <c r="L26" s="51"/>
-      <c r="M26" s="51"/>
-      <c r="N26" s="51"/>
-      <c r="O26" s="51"/>
-      <c r="P26" s="51"/>
-      <c r="Q26" s="51"/>
-      <c r="R26" s="51"/>
-      <c r="S26" s="51"/>
-      <c r="T26" s="51"/>
-      <c r="U26" s="51"/>
-      <c r="V26" s="51"/>
-      <c r="W26" s="51"/>
-      <c r="X26" s="51"/>
-      <c r="Y26" s="51"/>
-      <c r="Z26" s="51"/>
-      <c r="AA26" s="51"/>
-      <c r="AB26" s="51"/>
-      <c r="AC26" s="51"/>
-      <c r="AD26" s="51"/>
-      <c r="AE26" s="51"/>
-      <c r="AF26" s="51"/>
-      <c r="AG26" s="51"/>
-      <c r="AH26" s="51"/>
-      <c r="AI26" s="51"/>
-      <c r="AJ26" s="51"/>
-      <c r="AK26" s="51"/>
-      <c r="AL26" s="51"/>
-      <c r="AM26" s="51"/>
-      <c r="AN26" s="51"/>
-      <c r="AO26" s="51"/>
-      <c r="AP26" s="51"/>
-      <c r="AQ26" s="51"/>
-      <c r="AR26" s="52"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="38"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="38"/>
+      <c r="Q26" s="38"/>
+      <c r="R26" s="38"/>
+      <c r="S26" s="38"/>
+      <c r="T26" s="38"/>
+      <c r="U26" s="38"/>
+      <c r="V26" s="38"/>
+      <c r="W26" s="38"/>
+      <c r="X26" s="38"/>
+      <c r="Y26" s="38"/>
+      <c r="Z26" s="38"/>
+      <c r="AA26" s="38"/>
+      <c r="AB26" s="38"/>
+      <c r="AC26" s="38"/>
+      <c r="AD26" s="38"/>
+      <c r="AE26" s="38"/>
+      <c r="AF26" s="38"/>
+      <c r="AG26" s="38"/>
+      <c r="AH26" s="38"/>
+      <c r="AI26" s="38"/>
+      <c r="AJ26" s="38"/>
+      <c r="AK26" s="38"/>
+      <c r="AL26" s="38"/>
+      <c r="AM26" s="38"/>
+      <c r="AN26" s="38"/>
+      <c r="AO26" s="38"/>
+      <c r="AP26" s="38"/>
+      <c r="AQ26" s="38"/>
+      <c r="AR26" s="39"/>
       <c r="AS26" s="10"/>
       <c r="AT26" s="10"/>
       <c r="AU26" s="10"/>
@@ -2990,42 +2990,42 @@
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="51"/>
-      <c r="K27" s="51"/>
-      <c r="L27" s="51"/>
-      <c r="M27" s="51"/>
-      <c r="N27" s="51"/>
-      <c r="O27" s="51"/>
-      <c r="P27" s="51"/>
-      <c r="Q27" s="51"/>
-      <c r="R27" s="51"/>
-      <c r="S27" s="51"/>
-      <c r="T27" s="51"/>
-      <c r="U27" s="51"/>
-      <c r="V27" s="51"/>
-      <c r="W27" s="51"/>
-      <c r="X27" s="51"/>
-      <c r="Y27" s="51"/>
-      <c r="Z27" s="51"/>
-      <c r="AA27" s="51"/>
-      <c r="AB27" s="51"/>
-      <c r="AC27" s="51"/>
-      <c r="AD27" s="51"/>
-      <c r="AE27" s="51"/>
-      <c r="AF27" s="51"/>
-      <c r="AG27" s="51"/>
-      <c r="AH27" s="51"/>
-      <c r="AI27" s="51"/>
-      <c r="AJ27" s="51"/>
-      <c r="AK27" s="51"/>
-      <c r="AL27" s="51"/>
-      <c r="AM27" s="51"/>
-      <c r="AN27" s="51"/>
-      <c r="AO27" s="51"/>
-      <c r="AP27" s="51"/>
-      <c r="AQ27" s="51"/>
-      <c r="AR27" s="52"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="38"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="38"/>
+      <c r="M27" s="38"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="38"/>
+      <c r="P27" s="38"/>
+      <c r="Q27" s="38"/>
+      <c r="R27" s="38"/>
+      <c r="S27" s="38"/>
+      <c r="T27" s="38"/>
+      <c r="U27" s="38"/>
+      <c r="V27" s="38"/>
+      <c r="W27" s="38"/>
+      <c r="X27" s="38"/>
+      <c r="Y27" s="38"/>
+      <c r="Z27" s="38"/>
+      <c r="AA27" s="38"/>
+      <c r="AB27" s="38"/>
+      <c r="AC27" s="38"/>
+      <c r="AD27" s="38"/>
+      <c r="AE27" s="38"/>
+      <c r="AF27" s="38"/>
+      <c r="AG27" s="38"/>
+      <c r="AH27" s="38"/>
+      <c r="AI27" s="38"/>
+      <c r="AJ27" s="38"/>
+      <c r="AK27" s="38"/>
+      <c r="AL27" s="38"/>
+      <c r="AM27" s="38"/>
+      <c r="AN27" s="38"/>
+      <c r="AO27" s="38"/>
+      <c r="AP27" s="38"/>
+      <c r="AQ27" s="38"/>
+      <c r="AR27" s="39"/>
       <c r="AS27" s="10"/>
       <c r="AT27" s="10"/>
       <c r="AU27" s="10"/>
@@ -3044,42 +3044,42 @@
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="51"/>
-      <c r="K28" s="51"/>
-      <c r="L28" s="51"/>
-      <c r="M28" s="51"/>
-      <c r="N28" s="51"/>
-      <c r="O28" s="51"/>
-      <c r="P28" s="51"/>
-      <c r="Q28" s="51"/>
-      <c r="R28" s="51"/>
-      <c r="S28" s="51"/>
-      <c r="T28" s="51"/>
-      <c r="U28" s="51"/>
-      <c r="V28" s="51"/>
-      <c r="W28" s="51"/>
-      <c r="X28" s="51"/>
-      <c r="Y28" s="51"/>
-      <c r="Z28" s="51"/>
-      <c r="AA28" s="51"/>
-      <c r="AB28" s="51"/>
-      <c r="AC28" s="51"/>
-      <c r="AD28" s="51"/>
-      <c r="AE28" s="51"/>
-      <c r="AF28" s="51"/>
-      <c r="AG28" s="51"/>
-      <c r="AH28" s="51"/>
-      <c r="AI28" s="51"/>
-      <c r="AJ28" s="51"/>
-      <c r="AK28" s="51"/>
-      <c r="AL28" s="51"/>
-      <c r="AM28" s="51"/>
-      <c r="AN28" s="51"/>
-      <c r="AO28" s="51"/>
-      <c r="AP28" s="51"/>
-      <c r="AQ28" s="51"/>
-      <c r="AR28" s="52"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="38"/>
+      <c r="N28" s="38"/>
+      <c r="O28" s="38"/>
+      <c r="P28" s="38"/>
+      <c r="Q28" s="38"/>
+      <c r="R28" s="38"/>
+      <c r="S28" s="38"/>
+      <c r="T28" s="38"/>
+      <c r="U28" s="38"/>
+      <c r="V28" s="38"/>
+      <c r="W28" s="38"/>
+      <c r="X28" s="38"/>
+      <c r="Y28" s="38"/>
+      <c r="Z28" s="38"/>
+      <c r="AA28" s="38"/>
+      <c r="AB28" s="38"/>
+      <c r="AC28" s="38"/>
+      <c r="AD28" s="38"/>
+      <c r="AE28" s="38"/>
+      <c r="AF28" s="38"/>
+      <c r="AG28" s="38"/>
+      <c r="AH28" s="38"/>
+      <c r="AI28" s="38"/>
+      <c r="AJ28" s="38"/>
+      <c r="AK28" s="38"/>
+      <c r="AL28" s="38"/>
+      <c r="AM28" s="38"/>
+      <c r="AN28" s="38"/>
+      <c r="AO28" s="38"/>
+      <c r="AP28" s="38"/>
+      <c r="AQ28" s="38"/>
+      <c r="AR28" s="39"/>
       <c r="AS28" s="6"/>
       <c r="AT28" s="6"/>
       <c r="AU28" s="6"/>
@@ -3098,42 +3098,42 @@
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
-      <c r="I29" s="53"/>
-      <c r="J29" s="54"/>
-      <c r="K29" s="54"/>
-      <c r="L29" s="54"/>
-      <c r="M29" s="54"/>
-      <c r="N29" s="54"/>
-      <c r="O29" s="54"/>
-      <c r="P29" s="54"/>
-      <c r="Q29" s="54"/>
-      <c r="R29" s="54"/>
-      <c r="S29" s="54"/>
-      <c r="T29" s="54"/>
-      <c r="U29" s="54"/>
-      <c r="V29" s="54"/>
-      <c r="W29" s="54"/>
-      <c r="X29" s="54"/>
-      <c r="Y29" s="54"/>
-      <c r="Z29" s="54"/>
-      <c r="AA29" s="54"/>
-      <c r="AB29" s="54"/>
-      <c r="AC29" s="54"/>
-      <c r="AD29" s="54"/>
-      <c r="AE29" s="54"/>
-      <c r="AF29" s="54"/>
-      <c r="AG29" s="54"/>
-      <c r="AH29" s="54"/>
-      <c r="AI29" s="54"/>
-      <c r="AJ29" s="54"/>
-      <c r="AK29" s="54"/>
-      <c r="AL29" s="54"/>
-      <c r="AM29" s="54"/>
-      <c r="AN29" s="54"/>
-      <c r="AO29" s="54"/>
-      <c r="AP29" s="54"/>
-      <c r="AQ29" s="54"/>
-      <c r="AR29" s="55"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="41"/>
+      <c r="K29" s="41"/>
+      <c r="L29" s="41"/>
+      <c r="M29" s="41"/>
+      <c r="N29" s="41"/>
+      <c r="O29" s="41"/>
+      <c r="P29" s="41"/>
+      <c r="Q29" s="41"/>
+      <c r="R29" s="41"/>
+      <c r="S29" s="41"/>
+      <c r="T29" s="41"/>
+      <c r="U29" s="41"/>
+      <c r="V29" s="41"/>
+      <c r="W29" s="41"/>
+      <c r="X29" s="41"/>
+      <c r="Y29" s="41"/>
+      <c r="Z29" s="41"/>
+      <c r="AA29" s="41"/>
+      <c r="AB29" s="41"/>
+      <c r="AC29" s="41"/>
+      <c r="AD29" s="41"/>
+      <c r="AE29" s="41"/>
+      <c r="AF29" s="41"/>
+      <c r="AG29" s="41"/>
+      <c r="AH29" s="41"/>
+      <c r="AI29" s="41"/>
+      <c r="AJ29" s="41"/>
+      <c r="AK29" s="41"/>
+      <c r="AL29" s="41"/>
+      <c r="AM29" s="41"/>
+      <c r="AN29" s="41"/>
+      <c r="AO29" s="41"/>
+      <c r="AP29" s="41"/>
+      <c r="AQ29" s="41"/>
+      <c r="AR29" s="42"/>
       <c r="AS29" s="6"/>
       <c r="AT29" s="6"/>
       <c r="AU29" s="6"/>
@@ -3905,28 +3905,28 @@
       <c r="AC45" s="6"/>
       <c r="AD45" s="6"/>
       <c r="AE45" s="6"/>
-      <c r="AF45" s="29" t="s">
+      <c r="AF45" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="AG45" s="29"/>
-      <c r="AH45" s="29"/>
-      <c r="AI45" s="29"/>
-      <c r="AJ45" s="29"/>
-      <c r="AK45" s="29"/>
-      <c r="AL45" s="42"/>
-      <c r="AM45" s="42"/>
-      <c r="AN45" s="42"/>
-      <c r="AO45" s="42"/>
-      <c r="AP45" s="42"/>
-      <c r="AQ45" s="42"/>
-      <c r="AR45" s="42"/>
-      <c r="AS45" s="42"/>
-      <c r="AT45" s="42"/>
-      <c r="AU45" s="42"/>
-      <c r="AV45" s="42"/>
-      <c r="AW45" s="42"/>
-      <c r="AX45" s="42"/>
-      <c r="AY45" s="42"/>
+      <c r="AG45" s="32"/>
+      <c r="AH45" s="32"/>
+      <c r="AI45" s="32"/>
+      <c r="AJ45" s="32"/>
+      <c r="AK45" s="32"/>
+      <c r="AL45" s="33"/>
+      <c r="AM45" s="33"/>
+      <c r="AN45" s="33"/>
+      <c r="AO45" s="33"/>
+      <c r="AP45" s="33"/>
+      <c r="AQ45" s="33"/>
+      <c r="AR45" s="33"/>
+      <c r="AS45" s="33"/>
+      <c r="AT45" s="33"/>
+      <c r="AU45" s="33"/>
+      <c r="AV45" s="33"/>
+      <c r="AW45" s="33"/>
+      <c r="AX45" s="33"/>
+      <c r="AY45" s="33"/>
       <c r="AZ45" s="7"/>
     </row>
     <row r="46" spans="1:52" ht="10.5" customHeight="1">
@@ -3961,26 +3961,26 @@
       <c r="AC46" s="6"/>
       <c r="AD46" s="6"/>
       <c r="AE46" s="6"/>
-      <c r="AF46" s="29"/>
-      <c r="AG46" s="29"/>
-      <c r="AH46" s="29"/>
-      <c r="AI46" s="29"/>
-      <c r="AJ46" s="29"/>
-      <c r="AK46" s="29"/>
-      <c r="AL46" s="42"/>
-      <c r="AM46" s="42"/>
-      <c r="AN46" s="42"/>
-      <c r="AO46" s="42"/>
-      <c r="AP46" s="42"/>
-      <c r="AQ46" s="42"/>
-      <c r="AR46" s="42"/>
-      <c r="AS46" s="42"/>
-      <c r="AT46" s="42"/>
-      <c r="AU46" s="42"/>
-      <c r="AV46" s="42"/>
-      <c r="AW46" s="42"/>
-      <c r="AX46" s="42"/>
-      <c r="AY46" s="42"/>
+      <c r="AF46" s="32"/>
+      <c r="AG46" s="32"/>
+      <c r="AH46" s="32"/>
+      <c r="AI46" s="32"/>
+      <c r="AJ46" s="32"/>
+      <c r="AK46" s="32"/>
+      <c r="AL46" s="33"/>
+      <c r="AM46" s="33"/>
+      <c r="AN46" s="33"/>
+      <c r="AO46" s="33"/>
+      <c r="AP46" s="33"/>
+      <c r="AQ46" s="33"/>
+      <c r="AR46" s="33"/>
+      <c r="AS46" s="33"/>
+      <c r="AT46" s="33"/>
+      <c r="AU46" s="33"/>
+      <c r="AV46" s="33"/>
+      <c r="AW46" s="33"/>
+      <c r="AX46" s="33"/>
+      <c r="AY46" s="33"/>
       <c r="AZ46" s="7"/>
     </row>
     <row r="47" spans="1:52" ht="10.5" customHeight="1">
@@ -4015,30 +4015,30 @@
       <c r="AC47" s="6"/>
       <c r="AD47" s="6"/>
       <c r="AE47" s="6"/>
-      <c r="AF47" s="29" t="s">
+      <c r="AF47" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="AG47" s="29"/>
-      <c r="AH47" s="29"/>
-      <c r="AI47" s="29"/>
-      <c r="AJ47" s="29"/>
-      <c r="AK47" s="29"/>
-      <c r="AL47" s="28">
+      <c r="AG47" s="32"/>
+      <c r="AH47" s="32"/>
+      <c r="AI47" s="32"/>
+      <c r="AJ47" s="32"/>
+      <c r="AK47" s="32"/>
+      <c r="AL47" s="43">
         <v>45566</v>
       </c>
-      <c r="AM47" s="28"/>
-      <c r="AN47" s="28"/>
-      <c r="AO47" s="28"/>
-      <c r="AP47" s="28"/>
-      <c r="AQ47" s="28"/>
-      <c r="AR47" s="28"/>
-      <c r="AS47" s="28"/>
-      <c r="AT47" s="28"/>
-      <c r="AU47" s="28"/>
-      <c r="AV47" s="28"/>
-      <c r="AW47" s="28"/>
-      <c r="AX47" s="28"/>
-      <c r="AY47" s="28"/>
+      <c r="AM47" s="43"/>
+      <c r="AN47" s="43"/>
+      <c r="AO47" s="43"/>
+      <c r="AP47" s="43"/>
+      <c r="AQ47" s="43"/>
+      <c r="AR47" s="43"/>
+      <c r="AS47" s="43"/>
+      <c r="AT47" s="43"/>
+      <c r="AU47" s="43"/>
+      <c r="AV47" s="43"/>
+      <c r="AW47" s="43"/>
+      <c r="AX47" s="43"/>
+      <c r="AY47" s="43"/>
       <c r="AZ47" s="7"/>
     </row>
     <row r="48" spans="1:52" ht="10.5" customHeight="1">
@@ -4073,26 +4073,26 @@
       <c r="AC48" s="6"/>
       <c r="AD48" s="6"/>
       <c r="AE48" s="6"/>
-      <c r="AF48" s="29"/>
-      <c r="AG48" s="29"/>
-      <c r="AH48" s="29"/>
-      <c r="AI48" s="29"/>
-      <c r="AJ48" s="29"/>
-      <c r="AK48" s="29"/>
-      <c r="AL48" s="28"/>
-      <c r="AM48" s="28"/>
-      <c r="AN48" s="28"/>
-      <c r="AO48" s="28"/>
-      <c r="AP48" s="28"/>
-      <c r="AQ48" s="28"/>
-      <c r="AR48" s="28"/>
-      <c r="AS48" s="28"/>
-      <c r="AT48" s="28"/>
-      <c r="AU48" s="28"/>
-      <c r="AV48" s="28"/>
-      <c r="AW48" s="28"/>
-      <c r="AX48" s="28"/>
-      <c r="AY48" s="28"/>
+      <c r="AF48" s="32"/>
+      <c r="AG48" s="32"/>
+      <c r="AH48" s="32"/>
+      <c r="AI48" s="32"/>
+      <c r="AJ48" s="32"/>
+      <c r="AK48" s="32"/>
+      <c r="AL48" s="43"/>
+      <c r="AM48" s="43"/>
+      <c r="AN48" s="43"/>
+      <c r="AO48" s="43"/>
+      <c r="AP48" s="43"/>
+      <c r="AQ48" s="43"/>
+      <c r="AR48" s="43"/>
+      <c r="AS48" s="43"/>
+      <c r="AT48" s="43"/>
+      <c r="AU48" s="43"/>
+      <c r="AV48" s="43"/>
+      <c r="AW48" s="43"/>
+      <c r="AX48" s="43"/>
+      <c r="AY48" s="43"/>
       <c r="AZ48" s="7"/>
     </row>
     <row r="49" spans="1:52" ht="12" customHeight="1">
@@ -4127,30 +4127,30 @@
       <c r="AC49" s="6"/>
       <c r="AD49" s="6"/>
       <c r="AE49" s="6"/>
-      <c r="AF49" s="30" t="s">
+      <c r="AF49" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="AG49" s="31"/>
-      <c r="AH49" s="31"/>
-      <c r="AI49" s="31"/>
-      <c r="AJ49" s="31"/>
-      <c r="AK49" s="32"/>
-      <c r="AL49" s="36" t="s">
+      <c r="AG49" s="45"/>
+      <c r="AH49" s="45"/>
+      <c r="AI49" s="45"/>
+      <c r="AJ49" s="45"/>
+      <c r="AK49" s="46"/>
+      <c r="AL49" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="AM49" s="37"/>
-      <c r="AN49" s="37"/>
-      <c r="AO49" s="37"/>
-      <c r="AP49" s="37"/>
-      <c r="AQ49" s="37"/>
-      <c r="AR49" s="37"/>
-      <c r="AS49" s="37"/>
-      <c r="AT49" s="37"/>
-      <c r="AU49" s="37"/>
-      <c r="AV49" s="37"/>
-      <c r="AW49" s="37"/>
-      <c r="AX49" s="37"/>
-      <c r="AY49" s="38"/>
+      <c r="AM49" s="51"/>
+      <c r="AN49" s="51"/>
+      <c r="AO49" s="51"/>
+      <c r="AP49" s="51"/>
+      <c r="AQ49" s="51"/>
+      <c r="AR49" s="51"/>
+      <c r="AS49" s="51"/>
+      <c r="AT49" s="51"/>
+      <c r="AU49" s="51"/>
+      <c r="AV49" s="51"/>
+      <c r="AW49" s="51"/>
+      <c r="AX49" s="51"/>
+      <c r="AY49" s="52"/>
       <c r="AZ49" s="7"/>
     </row>
     <row r="50" spans="1:52" ht="12" customHeight="1">
@@ -4185,26 +4185,26 @@
       <c r="AC50" s="6"/>
       <c r="AD50" s="6"/>
       <c r="AE50" s="6"/>
-      <c r="AF50" s="33"/>
-      <c r="AG50" s="34"/>
-      <c r="AH50" s="34"/>
-      <c r="AI50" s="34"/>
-      <c r="AJ50" s="34"/>
-      <c r="AK50" s="35"/>
-      <c r="AL50" s="39"/>
-      <c r="AM50" s="40"/>
-      <c r="AN50" s="40"/>
-      <c r="AO50" s="40"/>
-      <c r="AP50" s="40"/>
-      <c r="AQ50" s="40"/>
-      <c r="AR50" s="40"/>
-      <c r="AS50" s="40"/>
-      <c r="AT50" s="40"/>
-      <c r="AU50" s="40"/>
-      <c r="AV50" s="40"/>
-      <c r="AW50" s="40"/>
-      <c r="AX50" s="40"/>
-      <c r="AY50" s="41"/>
+      <c r="AF50" s="47"/>
+      <c r="AG50" s="48"/>
+      <c r="AH50" s="48"/>
+      <c r="AI50" s="48"/>
+      <c r="AJ50" s="48"/>
+      <c r="AK50" s="49"/>
+      <c r="AL50" s="53"/>
+      <c r="AM50" s="54"/>
+      <c r="AN50" s="54"/>
+      <c r="AO50" s="54"/>
+      <c r="AP50" s="54"/>
+      <c r="AQ50" s="54"/>
+      <c r="AR50" s="54"/>
+      <c r="AS50" s="54"/>
+      <c r="AT50" s="54"/>
+      <c r="AU50" s="54"/>
+      <c r="AV50" s="54"/>
+      <c r="AW50" s="54"/>
+      <c r="AX50" s="54"/>
+      <c r="AY50" s="55"/>
       <c r="AZ50" s="7"/>
     </row>
     <row r="51" spans="1:52">
@@ -4317,17 +4317,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B3:L4"/>
-    <mergeCell ref="M3:P4"/>
-    <mergeCell ref="AF3:AK4"/>
-    <mergeCell ref="AL3:AY4"/>
-    <mergeCell ref="I16:AR29"/>
     <mergeCell ref="AL47:AY48"/>
     <mergeCell ref="AF47:AK48"/>
     <mergeCell ref="AF49:AK50"/>
     <mergeCell ref="AL49:AY50"/>
     <mergeCell ref="AF45:AK46"/>
     <mergeCell ref="AL45:AY46"/>
+    <mergeCell ref="B3:L4"/>
+    <mergeCell ref="M3:P4"/>
+    <mergeCell ref="AF3:AK4"/>
+    <mergeCell ref="AL3:AY4"/>
+    <mergeCell ref="I16:AR29"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.59055118110236227" right="0.39370078740157483" top="0.59055118110236227" bottom="0.59055118110236227" header="0.39370078740157483" footer="0.39370078740157483"/>
@@ -4353,240 +4353,240 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:52" ht="10.5" customHeight="1" thickTop="1">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
-      <c r="K1" s="64"/>
-      <c r="L1" s="64"/>
-      <c r="M1" s="64"/>
-      <c r="N1" s="64"/>
-      <c r="O1" s="64"/>
-      <c r="P1" s="64"/>
-      <c r="Q1" s="64"/>
-      <c r="R1" s="64"/>
-      <c r="S1" s="64"/>
-      <c r="T1" s="64"/>
-      <c r="U1" s="64"/>
-      <c r="V1" s="64"/>
-      <c r="W1" s="64"/>
-      <c r="X1" s="64"/>
-      <c r="Y1" s="64"/>
-      <c r="Z1" s="64"/>
-      <c r="AA1" s="64"/>
-      <c r="AB1" s="64"/>
-      <c r="AC1" s="64"/>
-      <c r="AD1" s="64"/>
-      <c r="AE1" s="64"/>
-      <c r="AF1" s="64"/>
-      <c r="AG1" s="64"/>
-      <c r="AH1" s="64"/>
-      <c r="AI1" s="64"/>
-      <c r="AJ1" s="64"/>
-      <c r="AK1" s="64"/>
-      <c r="AL1" s="64"/>
-      <c r="AM1" s="64"/>
-      <c r="AN1" s="64"/>
-      <c r="AO1" s="64"/>
-      <c r="AP1" s="64"/>
-      <c r="AQ1" s="64"/>
-      <c r="AR1" s="64"/>
-      <c r="AS1" s="64"/>
-      <c r="AT1" s="64"/>
-      <c r="AU1" s="64"/>
-      <c r="AV1" s="64"/>
-      <c r="AW1" s="64"/>
-      <c r="AX1" s="64"/>
-      <c r="AY1" s="64"/>
-      <c r="AZ1" s="65"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
+      <c r="Z1" s="59"/>
+      <c r="AA1" s="59"/>
+      <c r="AB1" s="59"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="59"/>
+      <c r="AF1" s="59"/>
+      <c r="AG1" s="59"/>
+      <c r="AH1" s="59"/>
+      <c r="AI1" s="59"/>
+      <c r="AJ1" s="59"/>
+      <c r="AK1" s="59"/>
+      <c r="AL1" s="59"/>
+      <c r="AM1" s="59"/>
+      <c r="AN1" s="59"/>
+      <c r="AO1" s="59"/>
+      <c r="AP1" s="59"/>
+      <c r="AQ1" s="59"/>
+      <c r="AR1" s="59"/>
+      <c r="AS1" s="59"/>
+      <c r="AT1" s="59"/>
+      <c r="AU1" s="59"/>
+      <c r="AV1" s="59"/>
+      <c r="AW1" s="59"/>
+      <c r="AX1" s="59"/>
+      <c r="AY1" s="59"/>
+      <c r="AZ1" s="60"/>
     </row>
     <row r="2" spans="1:52" ht="10.5" customHeight="1" thickBot="1">
-      <c r="A2" s="66"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
-      <c r="K2" s="67"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="67"/>
-      <c r="N2" s="67"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="67"/>
-      <c r="Q2" s="67"/>
-      <c r="R2" s="67"/>
-      <c r="S2" s="67"/>
-      <c r="T2" s="67"/>
-      <c r="U2" s="67"/>
-      <c r="V2" s="67"/>
-      <c r="W2" s="67"/>
-      <c r="X2" s="67"/>
-      <c r="Y2" s="67"/>
-      <c r="Z2" s="67"/>
-      <c r="AA2" s="67"/>
-      <c r="AB2" s="67"/>
-      <c r="AC2" s="67"/>
-      <c r="AD2" s="67"/>
-      <c r="AE2" s="67"/>
-      <c r="AF2" s="67"/>
-      <c r="AG2" s="67"/>
-      <c r="AH2" s="67"/>
-      <c r="AI2" s="67"/>
-      <c r="AJ2" s="67"/>
-      <c r="AK2" s="67"/>
-      <c r="AL2" s="67"/>
-      <c r="AM2" s="67"/>
-      <c r="AN2" s="67"/>
-      <c r="AO2" s="67"/>
-      <c r="AP2" s="67"/>
-      <c r="AQ2" s="67"/>
-      <c r="AR2" s="67"/>
-      <c r="AS2" s="67"/>
-      <c r="AT2" s="67"/>
-      <c r="AU2" s="67"/>
-      <c r="AV2" s="67"/>
-      <c r="AW2" s="67"/>
-      <c r="AX2" s="67"/>
-      <c r="AY2" s="67"/>
-      <c r="AZ2" s="68"/>
+      <c r="A2" s="61"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
+      <c r="H2" s="62"/>
+      <c r="I2" s="62"/>
+      <c r="J2" s="62"/>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
+      <c r="Q2" s="62"/>
+      <c r="R2" s="62"/>
+      <c r="S2" s="62"/>
+      <c r="T2" s="62"/>
+      <c r="U2" s="62"/>
+      <c r="V2" s="62"/>
+      <c r="W2" s="62"/>
+      <c r="X2" s="62"/>
+      <c r="Y2" s="62"/>
+      <c r="Z2" s="62"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
+      <c r="AC2" s="62"/>
+      <c r="AD2" s="62"/>
+      <c r="AE2" s="62"/>
+      <c r="AF2" s="62"/>
+      <c r="AG2" s="62"/>
+      <c r="AH2" s="62"/>
+      <c r="AI2" s="62"/>
+      <c r="AJ2" s="62"/>
+      <c r="AK2" s="62"/>
+      <c r="AL2" s="62"/>
+      <c r="AM2" s="62"/>
+      <c r="AN2" s="62"/>
+      <c r="AO2" s="62"/>
+      <c r="AP2" s="62"/>
+      <c r="AQ2" s="62"/>
+      <c r="AR2" s="62"/>
+      <c r="AS2" s="62"/>
+      <c r="AT2" s="62"/>
+      <c r="AU2" s="62"/>
+      <c r="AV2" s="62"/>
+      <c r="AW2" s="62"/>
+      <c r="AX2" s="62"/>
+      <c r="AY2" s="62"/>
+      <c r="AZ2" s="63"/>
     </row>
     <row r="3" spans="1:52" ht="10.199999999999999" thickTop="1"/>
     <row r="4" spans="1:52" ht="12">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="60"/>
-      <c r="C4" s="58" t="s">
+      <c r="B4" s="68"/>
+      <c r="C4" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="59"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="58" t="s">
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="59"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="58" t="s">
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59"/>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59"/>
-      <c r="Q4" s="59"/>
-      <c r="R4" s="59"/>
-      <c r="S4" s="59"/>
-      <c r="T4" s="60"/>
-      <c r="U4" s="58" t="s">
+      <c r="L4" s="67"/>
+      <c r="M4" s="67"/>
+      <c r="N4" s="67"/>
+      <c r="O4" s="67"/>
+      <c r="P4" s="67"/>
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="67"/>
+      <c r="T4" s="68"/>
+      <c r="U4" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="V4" s="59"/>
-      <c r="W4" s="59"/>
-      <c r="X4" s="59"/>
-      <c r="Y4" s="59"/>
-      <c r="Z4" s="59"/>
-      <c r="AA4" s="59"/>
-      <c r="AB4" s="59"/>
-      <c r="AC4" s="59"/>
-      <c r="AD4" s="59"/>
-      <c r="AE4" s="59"/>
-      <c r="AF4" s="59"/>
-      <c r="AG4" s="59"/>
-      <c r="AH4" s="59"/>
-      <c r="AI4" s="59"/>
-      <c r="AJ4" s="59"/>
-      <c r="AK4" s="59"/>
-      <c r="AL4" s="59"/>
-      <c r="AM4" s="59"/>
-      <c r="AN4" s="59"/>
-      <c r="AO4" s="59"/>
-      <c r="AP4" s="59"/>
-      <c r="AQ4" s="59"/>
-      <c r="AR4" s="59"/>
-      <c r="AS4" s="59"/>
-      <c r="AT4" s="59"/>
-      <c r="AU4" s="59"/>
-      <c r="AV4" s="59"/>
-      <c r="AW4" s="59"/>
-      <c r="AX4" s="59"/>
-      <c r="AY4" s="59"/>
-      <c r="AZ4" s="60"/>
+      <c r="V4" s="67"/>
+      <c r="W4" s="67"/>
+      <c r="X4" s="67"/>
+      <c r="Y4" s="67"/>
+      <c r="Z4" s="67"/>
+      <c r="AA4" s="67"/>
+      <c r="AB4" s="67"/>
+      <c r="AC4" s="67"/>
+      <c r="AD4" s="67"/>
+      <c r="AE4" s="67"/>
+      <c r="AF4" s="67"/>
+      <c r="AG4" s="67"/>
+      <c r="AH4" s="67"/>
+      <c r="AI4" s="67"/>
+      <c r="AJ4" s="67"/>
+      <c r="AK4" s="67"/>
+      <c r="AL4" s="67"/>
+      <c r="AM4" s="67"/>
+      <c r="AN4" s="67"/>
+      <c r="AO4" s="67"/>
+      <c r="AP4" s="67"/>
+      <c r="AQ4" s="67"/>
+      <c r="AR4" s="67"/>
+      <c r="AS4" s="67"/>
+      <c r="AT4" s="67"/>
+      <c r="AU4" s="67"/>
+      <c r="AV4" s="67"/>
+      <c r="AW4" s="67"/>
+      <c r="AX4" s="67"/>
+      <c r="AY4" s="67"/>
+      <c r="AZ4" s="68"/>
     </row>
     <row r="5" spans="1:52" ht="12">
-      <c r="A5" s="61">
+      <c r="A5" s="69">
         <f t="shared" ref="A5:A46" si="0">ROW()-4</f>
         <v>1</v>
       </c>
-      <c r="B5" s="61"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="62"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61"/>
-      <c r="K5" s="61" t="s">
+      <c r="B5" s="69"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="61"/>
-      <c r="M5" s="61"/>
-      <c r="N5" s="61"/>
-      <c r="O5" s="61"/>
-      <c r="P5" s="61"/>
-      <c r="Q5" s="61"/>
-      <c r="R5" s="61"/>
-      <c r="S5" s="61"/>
-      <c r="T5" s="61"/>
-      <c r="U5" s="61" t="s">
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="69"/>
+      <c r="Q5" s="69"/>
+      <c r="R5" s="69"/>
+      <c r="S5" s="69"/>
+      <c r="T5" s="69"/>
+      <c r="U5" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="V5" s="61"/>
-      <c r="W5" s="61"/>
-      <c r="X5" s="61"/>
-      <c r="Y5" s="61"/>
-      <c r="Z5" s="61"/>
-      <c r="AA5" s="61"/>
-      <c r="AB5" s="61"/>
-      <c r="AC5" s="61"/>
-      <c r="AD5" s="61"/>
-      <c r="AE5" s="61"/>
-      <c r="AF5" s="61"/>
-      <c r="AG5" s="61"/>
-      <c r="AH5" s="61"/>
-      <c r="AI5" s="61"/>
-      <c r="AJ5" s="61"/>
-      <c r="AK5" s="61"/>
-      <c r="AL5" s="61"/>
-      <c r="AM5" s="61"/>
-      <c r="AN5" s="61"/>
-      <c r="AO5" s="61"/>
-      <c r="AP5" s="61"/>
-      <c r="AQ5" s="61"/>
-      <c r="AR5" s="61"/>
-      <c r="AS5" s="61"/>
-      <c r="AT5" s="61"/>
-      <c r="AU5" s="61"/>
-      <c r="AV5" s="61"/>
-      <c r="AW5" s="61"/>
-      <c r="AX5" s="61"/>
-      <c r="AY5" s="61"/>
-      <c r="AZ5" s="61"/>
+      <c r="V5" s="69"/>
+      <c r="W5" s="69"/>
+      <c r="X5" s="69"/>
+      <c r="Y5" s="69"/>
+      <c r="Z5" s="69"/>
+      <c r="AA5" s="69"/>
+      <c r="AB5" s="69"/>
+      <c r="AC5" s="69"/>
+      <c r="AD5" s="69"/>
+      <c r="AE5" s="69"/>
+      <c r="AF5" s="69"/>
+      <c r="AG5" s="69"/>
+      <c r="AH5" s="69"/>
+      <c r="AI5" s="69"/>
+      <c r="AJ5" s="69"/>
+      <c r="AK5" s="69"/>
+      <c r="AL5" s="69"/>
+      <c r="AM5" s="69"/>
+      <c r="AN5" s="69"/>
+      <c r="AO5" s="69"/>
+      <c r="AP5" s="69"/>
+      <c r="AQ5" s="69"/>
+      <c r="AR5" s="69"/>
+      <c r="AS5" s="69"/>
+      <c r="AT5" s="69"/>
+      <c r="AU5" s="69"/>
+      <c r="AV5" s="69"/>
+      <c r="AW5" s="69"/>
+      <c r="AX5" s="69"/>
+      <c r="AY5" s="69"/>
+      <c r="AZ5" s="69"/>
     </row>
     <row r="6" spans="1:52" ht="12">
       <c r="A6" s="56">
@@ -6869,64 +6869,256 @@
       <c r="AZ45" s="56"/>
     </row>
     <row r="46" spans="1:52" ht="12">
-      <c r="A46" s="69">
+      <c r="A46" s="64">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B46" s="69"/>
-      <c r="C46" s="70"/>
-      <c r="D46" s="70"/>
-      <c r="E46" s="70"/>
-      <c r="F46" s="70"/>
-      <c r="G46" s="69"/>
-      <c r="H46" s="69"/>
-      <c r="I46" s="69"/>
-      <c r="J46" s="69"/>
-      <c r="K46" s="69"/>
-      <c r="L46" s="69"/>
-      <c r="M46" s="69"/>
-      <c r="N46" s="69"/>
-      <c r="O46" s="69"/>
-      <c r="P46" s="69"/>
-      <c r="Q46" s="69"/>
-      <c r="R46" s="69"/>
-      <c r="S46" s="69"/>
-      <c r="T46" s="69"/>
-      <c r="U46" s="69"/>
-      <c r="V46" s="69"/>
-      <c r="W46" s="69"/>
-      <c r="X46" s="69"/>
-      <c r="Y46" s="69"/>
-      <c r="Z46" s="69"/>
-      <c r="AA46" s="69"/>
-      <c r="AB46" s="69"/>
-      <c r="AC46" s="69"/>
-      <c r="AD46" s="69"/>
-      <c r="AE46" s="69"/>
-      <c r="AF46" s="69"/>
-      <c r="AG46" s="69"/>
-      <c r="AH46" s="69"/>
-      <c r="AI46" s="69"/>
-      <c r="AJ46" s="69"/>
-      <c r="AK46" s="69"/>
-      <c r="AL46" s="69"/>
-      <c r="AM46" s="69"/>
-      <c r="AN46" s="69"/>
-      <c r="AO46" s="69"/>
-      <c r="AP46" s="69"/>
-      <c r="AQ46" s="69"/>
-      <c r="AR46" s="69"/>
-      <c r="AS46" s="69"/>
-      <c r="AT46" s="69"/>
-      <c r="AU46" s="69"/>
-      <c r="AV46" s="69"/>
-      <c r="AW46" s="69"/>
-      <c r="AX46" s="69"/>
-      <c r="AY46" s="69"/>
-      <c r="AZ46" s="69"/>
+      <c r="B46" s="64"/>
+      <c r="C46" s="65"/>
+      <c r="D46" s="65"/>
+      <c r="E46" s="65"/>
+      <c r="F46" s="65"/>
+      <c r="G46" s="64"/>
+      <c r="H46" s="64"/>
+      <c r="I46" s="64"/>
+      <c r="J46" s="64"/>
+      <c r="K46" s="64"/>
+      <c r="L46" s="64"/>
+      <c r="M46" s="64"/>
+      <c r="N46" s="64"/>
+      <c r="O46" s="64"/>
+      <c r="P46" s="64"/>
+      <c r="Q46" s="64"/>
+      <c r="R46" s="64"/>
+      <c r="S46" s="64"/>
+      <c r="T46" s="64"/>
+      <c r="U46" s="64"/>
+      <c r="V46" s="64"/>
+      <c r="W46" s="64"/>
+      <c r="X46" s="64"/>
+      <c r="Y46" s="64"/>
+      <c r="Z46" s="64"/>
+      <c r="AA46" s="64"/>
+      <c r="AB46" s="64"/>
+      <c r="AC46" s="64"/>
+      <c r="AD46" s="64"/>
+      <c r="AE46" s="64"/>
+      <c r="AF46" s="64"/>
+      <c r="AG46" s="64"/>
+      <c r="AH46" s="64"/>
+      <c r="AI46" s="64"/>
+      <c r="AJ46" s="64"/>
+      <c r="AK46" s="64"/>
+      <c r="AL46" s="64"/>
+      <c r="AM46" s="64"/>
+      <c r="AN46" s="64"/>
+      <c r="AO46" s="64"/>
+      <c r="AP46" s="64"/>
+      <c r="AQ46" s="64"/>
+      <c r="AR46" s="64"/>
+      <c r="AS46" s="64"/>
+      <c r="AT46" s="64"/>
+      <c r="AU46" s="64"/>
+      <c r="AV46" s="64"/>
+      <c r="AW46" s="64"/>
+      <c r="AX46" s="64"/>
+      <c r="AY46" s="64"/>
+      <c r="AZ46" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="216">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="K6:T6"/>
+    <mergeCell ref="U6:AZ6"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="G5:J5"/>
+    <mergeCell ref="K4:T4"/>
+    <mergeCell ref="K5:T5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="U4:AZ4"/>
+    <mergeCell ref="U5:AZ5"/>
+    <mergeCell ref="U7:AZ7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="K8:T8"/>
+    <mergeCell ref="U8:AZ8"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="K7:T7"/>
+    <mergeCell ref="U9:AZ9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="K10:T10"/>
+    <mergeCell ref="U10:AZ10"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="K9:T9"/>
+    <mergeCell ref="U11:AZ11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="K12:T12"/>
+    <mergeCell ref="U12:AZ12"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="K11:T11"/>
+    <mergeCell ref="U13:AZ13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="K14:T14"/>
+    <mergeCell ref="U14:AZ14"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="K13:T13"/>
+    <mergeCell ref="U15:AZ15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="K16:T16"/>
+    <mergeCell ref="U16:AZ16"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="K15:T15"/>
+    <mergeCell ref="U17:AZ17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="K18:T18"/>
+    <mergeCell ref="U18:AZ18"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="K17:T17"/>
+    <mergeCell ref="U19:AZ19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="K20:T20"/>
+    <mergeCell ref="U20:AZ20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="K19:T19"/>
+    <mergeCell ref="U21:AZ21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="K22:T22"/>
+    <mergeCell ref="U22:AZ22"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="K21:T21"/>
+    <mergeCell ref="U23:AZ23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="K24:T24"/>
+    <mergeCell ref="U24:AZ24"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="K23:T23"/>
+    <mergeCell ref="U25:AZ25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="K26:T26"/>
+    <mergeCell ref="U26:AZ26"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="K25:T25"/>
+    <mergeCell ref="U27:AZ27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="K28:T28"/>
+    <mergeCell ref="U28:AZ28"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="K27:T27"/>
+    <mergeCell ref="U29:AZ29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="G30:J30"/>
+    <mergeCell ref="K30:T30"/>
+    <mergeCell ref="U30:AZ30"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="K29:T29"/>
+    <mergeCell ref="U31:AZ31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="K32:T32"/>
+    <mergeCell ref="U32:AZ32"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="G31:J31"/>
+    <mergeCell ref="K31:T31"/>
+    <mergeCell ref="U33:AZ33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="K34:T34"/>
+    <mergeCell ref="U34:AZ34"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="G33:J33"/>
+    <mergeCell ref="K33:T33"/>
+    <mergeCell ref="C41:F41"/>
+    <mergeCell ref="G41:J41"/>
+    <mergeCell ref="K41:T41"/>
+    <mergeCell ref="U35:AZ35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="K36:T36"/>
+    <mergeCell ref="U36:AZ36"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="K35:T35"/>
+    <mergeCell ref="K43:T43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="U37:AZ37"/>
+    <mergeCell ref="U38:AZ38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:F42"/>
+    <mergeCell ref="G42:J42"/>
+    <mergeCell ref="U39:AZ39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="G37:J37"/>
+    <mergeCell ref="K37:T37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="G38:J38"/>
+    <mergeCell ref="K38:T38"/>
+    <mergeCell ref="G40:J40"/>
+    <mergeCell ref="K40:T40"/>
+    <mergeCell ref="U40:AZ40"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="U41:AZ41"/>
+    <mergeCell ref="A41:B41"/>
     <mergeCell ref="G44:J44"/>
     <mergeCell ref="K44:T44"/>
     <mergeCell ref="C40:F40"/>
@@ -6951,198 +7143,6 @@
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="C43:F43"/>
     <mergeCell ref="G43:J43"/>
-    <mergeCell ref="K43:T43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:F44"/>
-    <mergeCell ref="U37:AZ37"/>
-    <mergeCell ref="U38:AZ38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:F42"/>
-    <mergeCell ref="G42:J42"/>
-    <mergeCell ref="U39:AZ39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="G37:J37"/>
-    <mergeCell ref="K37:T37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="G38:J38"/>
-    <mergeCell ref="K38:T38"/>
-    <mergeCell ref="G40:J40"/>
-    <mergeCell ref="K40:T40"/>
-    <mergeCell ref="U40:AZ40"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="U41:AZ41"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:F41"/>
-    <mergeCell ref="G41:J41"/>
-    <mergeCell ref="K41:T41"/>
-    <mergeCell ref="U35:AZ35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="G36:J36"/>
-    <mergeCell ref="K36:T36"/>
-    <mergeCell ref="U36:AZ36"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="G35:J35"/>
-    <mergeCell ref="K35:T35"/>
-    <mergeCell ref="U33:AZ33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="K34:T34"/>
-    <mergeCell ref="U34:AZ34"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="G33:J33"/>
-    <mergeCell ref="K33:T33"/>
-    <mergeCell ref="U31:AZ31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="K32:T32"/>
-    <mergeCell ref="U32:AZ32"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="C31:F31"/>
-    <mergeCell ref="G31:J31"/>
-    <mergeCell ref="K31:T31"/>
-    <mergeCell ref="U29:AZ29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="G30:J30"/>
-    <mergeCell ref="K30:T30"/>
-    <mergeCell ref="U30:AZ30"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="K29:T29"/>
-    <mergeCell ref="U27:AZ27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="K28:T28"/>
-    <mergeCell ref="U28:AZ28"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="K27:T27"/>
-    <mergeCell ref="U25:AZ25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="K26:T26"/>
-    <mergeCell ref="U26:AZ26"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="K25:T25"/>
-    <mergeCell ref="U23:AZ23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="K24:T24"/>
-    <mergeCell ref="U24:AZ24"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="K23:T23"/>
-    <mergeCell ref="U21:AZ21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="K22:T22"/>
-    <mergeCell ref="U22:AZ22"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="K21:T21"/>
-    <mergeCell ref="U19:AZ19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="K20:T20"/>
-    <mergeCell ref="U20:AZ20"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="K19:T19"/>
-    <mergeCell ref="U17:AZ17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="K18:T18"/>
-    <mergeCell ref="U18:AZ18"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="K17:T17"/>
-    <mergeCell ref="U15:AZ15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="K16:T16"/>
-    <mergeCell ref="U16:AZ16"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="K15:T15"/>
-    <mergeCell ref="U13:AZ13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="K14:T14"/>
-    <mergeCell ref="U14:AZ14"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="K13:T13"/>
-    <mergeCell ref="U11:AZ11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="K12:T12"/>
-    <mergeCell ref="U12:AZ12"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="K11:T11"/>
-    <mergeCell ref="U9:AZ9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="K10:T10"/>
-    <mergeCell ref="U10:AZ10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="K9:T9"/>
-    <mergeCell ref="U7:AZ7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="K8:T8"/>
-    <mergeCell ref="U8:AZ8"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="K7:T7"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="G6:J6"/>
-    <mergeCell ref="K6:T6"/>
-    <mergeCell ref="U6:AZ6"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="K4:T4"/>
-    <mergeCell ref="K5:T5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="U4:AZ4"/>
-    <mergeCell ref="U5:AZ5"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.59055118110236227" right="0.39370078740157483" top="0.59055118110236227" bottom="0.59055118110236227" header="0.39370078740157483" footer="0.39370078740157483"/>
@@ -7157,8 +7157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AZ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AL2" sqref="AL2:AT2"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BV39" sqref="BV39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="9.6"/>

</xml_diff>